<commit_message>
The parasitic resistance and inductance values are derived using FEM tool. The JPEG shows equivalent inverter circuit.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/IMMD Production/Test sonuçları/Kart A sonuçlar.xlsx
+++ b/Project/3501/Furkan/IMMD Production/Test sonuçları/Kart A sonuçlar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Sonuçları" sheetId="1" r:id="rId1"/>
@@ -748,7 +748,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="tr-TR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -812,7 +812,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="tr-TR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -994,7 +994,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="tr-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="495401200"/>
@@ -1053,7 +1053,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="tr-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="487229328"/>
@@ -1094,7 +1094,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="tr-TR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1108,7 +1108,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="tr-TR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1172,7 +1172,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="tr-TR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1354,7 +1354,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="tr-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="495401200"/>
@@ -1413,7 +1413,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="tr-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="487229328"/>
@@ -1454,7 +1454,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="tr-TR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1468,7 +1468,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="tr-TR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1703,7 +1703,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="tr-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="495401200"/>
@@ -1762,7 +1762,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="tr-TR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="487229328"/>
@@ -1781,7 +1781,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="tr-TR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3002,7 +3002,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5736,7 +5736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -6020,7 +6020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>

</xml_diff>